<commit_message>
feat: implement Item Gaps, Favicon, Manifest and Algorithm Docs
</commit_message>
<xml_diff>
--- a/public/packflow_template.xlsx
+++ b/public/packflow_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isbol\Documents\PROJECTS\P_PERSONALES\PackFlow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isbol\Documents\PROJECTS\P_PERSONALES\PackFlow\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0409BC-E6A7-4B7D-A033-BFD3626D3543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBD14F9-1049-4154-9505-1700EC614ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-7956" windowWidth="23232" windowHeight="14592" xr2:uid="{9389FDD1-BA8B-48DB-A85F-77195E465889}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Item Name</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Pipes</t>
+  </si>
+  <si>
+    <t>Gap length (m)</t>
+  </si>
+  <si>
+    <t>Gap Width (m)</t>
   </si>
 </sst>
 </file>
@@ -144,17 +150,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -204,9 +216,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{655E63EB-52A7-4C59-8D92-691DB53B6AB7}" name="Tabla1" displayName="Tabla1" ref="A2:H4" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A2:H4" xr:uid="{655E63EB-52A7-4C59-8D92-691DB53B6AB7}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{655E63EB-52A7-4C59-8D92-691DB53B6AB7}" name="Tabla1" displayName="Tabla1" ref="A2:J4" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:J4" xr:uid="{655E63EB-52A7-4C59-8D92-691DB53B6AB7}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A7EDDADD-50AD-44A1-87D0-87A5AB8D61CC}" name="Item Name" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{E0ED2AAB-11DC-4013-9A91-D9BCFF2DAB6F}" name="Length (m)" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{11682034-2343-4B22-9218-4E417972FFA0}" name="Width (m)" dataDxfId="7"/>
@@ -215,6 +227,8 @@
     <tableColumn id="6" xr3:uid="{745C49B6-FCEE-4833-AB6E-DEE56861BF61}" name="Qty" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{E4CBAB8B-DDE6-46EE-B3F5-86946D965C65}" name="Stockable (0/1)" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{FD6D7BB0-5050-4F86-BB26-25B9DD9E75F3}" name="Rotatable (0/1)" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{A4C90877-1E30-4602-BEA9-5FFC4926B607}" name="Gap length (m)" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{E9B8A0D7-0C31-4CED-AB51-E6B8B707FF9D}" name="Gap Width (m)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -540,102 +554,122 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>1.2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.8</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>1.7</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>450</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>0</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>1</v>
       </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>3.5</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.3</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>0.3</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>15</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>50</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>1</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>